<commit_message>
update: Started working on new Request type in SDE
</commit_message>
<xml_diff>
--- a/SDEaaS_sample_synopses_and_parameters.xlsx
+++ b/SDEaaS_sample_synopses_and_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ado.kontax\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Γιάννης\Documents\eclipse-workspace\SDE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D404ABA-AA14-4E3F-8BA0-2EDB65FCD15E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2767C81-957A-461B-8A5D-A2D3B37C886E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0EAD80D5-834A-43B5-80E7-787A33F4B58C}"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{0EAD80D5-834A-43B5-80E7-787A33F4B58C}"/>
   </bookViews>
   <sheets>
     <sheet name="Synopses" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>SynopsisID</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>keyField, ValueField, OperationMode, windowSize</t>
+  </si>
+  <si>
+    <t>request an estimation among multiple Synopses</t>
   </si>
 </sst>
 </file>
@@ -352,8 +355,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Υπερ-σύνδεση" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -450,8 +453,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9946CC44-A03B-4057-BA82-4C084AB27645}" name="Table16" displayName="Table16" ref="A1:C8" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:C8" xr:uid="{1C44254B-134C-4068-95A3-1E792984E53A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9946CC44-A03B-4057-BA82-4C084AB27645}" name="Table16" displayName="Table16" ref="A1:C9" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:C9" xr:uid="{1C44254B-134C-4068-95A3-1E792984E53A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5E797631-A6E9-40C7-BD47-66DD11E45078}" name="RequestID" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{3C291575-BEE6-47DF-808A-141DD3D2245E}" name="OperationType" dataDxfId="1"/>
@@ -462,7 +465,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -760,7 +763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC58821-3DCC-4CEB-BE8D-A46D559ECFB3}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A21" sqref="A21:A24"/>
     </sheetView>
   </sheetViews>
@@ -1157,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8748E1D5-41B4-4AF2-9826-1D90F64A5E40}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,9 +1260,15 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>

</xml_diff>

<commit_message>
feature: add new type of Request for estimating multiple Synopses
</commit_message>
<xml_diff>
--- a/SDEaaS_sample_synopses_and_parameters.xlsx
+++ b/SDEaaS_sample_synopses_and_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ado.kontax\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Γιάννης\Documents\eclipse-workspace\SDE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D404ABA-AA14-4E3F-8BA0-2EDB65FCD15E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2767C81-957A-461B-8A5D-A2D3B37C886E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0EAD80D5-834A-43B5-80E7-787A33F4B58C}"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{0EAD80D5-834A-43B5-80E7-787A33F4B58C}"/>
   </bookViews>
   <sheets>
     <sheet name="Synopses" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>SynopsisID</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>keyField, ValueField, OperationMode, windowSize</t>
+  </si>
+  <si>
+    <t>request an estimation among multiple Synopses</t>
   </si>
 </sst>
 </file>
@@ -352,8 +355,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Υπερ-σύνδεση" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -450,8 +453,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9946CC44-A03B-4057-BA82-4C084AB27645}" name="Table16" displayName="Table16" ref="A1:C8" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:C8" xr:uid="{1C44254B-134C-4068-95A3-1E792984E53A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9946CC44-A03B-4057-BA82-4C084AB27645}" name="Table16" displayName="Table16" ref="A1:C9" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:C9" xr:uid="{1C44254B-134C-4068-95A3-1E792984E53A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5E797631-A6E9-40C7-BD47-66DD11E45078}" name="RequestID" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{3C291575-BEE6-47DF-808A-141DD3D2245E}" name="OperationType" dataDxfId="1"/>
@@ -462,7 +465,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -760,7 +763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC58821-3DCC-4CEB-BE8D-A46D559ECFB3}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A21" sqref="A21:A24"/>
     </sheetView>
   </sheetViews>
@@ -1157,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8748E1D5-41B4-4AF2-9826-1D90F64A5E40}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,9 +1260,15 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>

</xml_diff>